<commit_message>
feat: múltiples items, pulgadas y descarga de imagen
- Dimensiones en pulgadas (in) en vez de cm
- Agregar múltiples productos al pedido con cantidades independientes
- Editar y quitar items de la lista
- Resumen en tabla con desglose por item y totales
- Botón de descargar resumen como imagen PNG
- Reemplaza html2canvas por html-to-image (compatible con oklch)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/public/mean-pack-template.xlsx
+++ b/public/mean-pack-template.xlsx
@@ -416,13 +416,13 @@
         <v>box_weight_kg</v>
       </c>
       <c r="E1" t="str">
-        <v>box_length_cm</v>
+        <v>box_length_in</v>
       </c>
       <c r="F1" t="str">
-        <v>box_width_cm</v>
+        <v>box_width_in</v>
       </c>
       <c r="G1" t="str">
-        <v>box_height_cm</v>
+        <v>box_height_in</v>
       </c>
       <c r="H1" t="str">
         <v>unit_weight_kg</v>
@@ -442,13 +442,13 @@
         <v>8.5</v>
       </c>
       <c r="E2">
-        <v>40</v>
+        <v>15.7</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>11.8</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>9.8</v>
       </c>
       <c r="H2">
         <v>0.41</v>
@@ -468,13 +468,13 @@
         <v>8.5</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>15.7</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>11.8</v>
       </c>
       <c r="G3">
-        <v>25</v>
+        <v>9.8</v>
       </c>
       <c r="H3">
         <v>0.41</v>
@@ -494,13 +494,13 @@
         <v>10.2</v>
       </c>
       <c r="E4">
-        <v>45</v>
+        <v>17.7</v>
       </c>
       <c r="F4">
-        <v>35</v>
+        <v>13.8</v>
       </c>
       <c r="G4">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>0.82</v>
@@ -520,13 +520,13 @@
         <v>10.2</v>
       </c>
       <c r="E5">
-        <v>45</v>
+        <v>17.7</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>13.8</v>
       </c>
       <c r="G5">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>0.82</v>
@@ -546,13 +546,13 @@
         <v>9.6</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>19.7</v>
       </c>
       <c r="F6">
-        <v>35</v>
+        <v>13.8</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>7.9</v>
       </c>
       <c r="H6">
         <v>1.15</v>
@@ -572,13 +572,13 @@
         <v>11</v>
       </c>
       <c r="E7">
-        <v>48</v>
+        <v>18.9</v>
       </c>
       <c r="F7">
-        <v>32</v>
+        <v>12.6</v>
       </c>
       <c r="G7">
-        <v>22</v>
+        <v>8.7</v>
       </c>
       <c r="H7">
         <v>0.7</v>
@@ -598,13 +598,13 @@
         <v>10.8</v>
       </c>
       <c r="E8">
-        <v>50</v>
+        <v>19.7</v>
       </c>
       <c r="F8">
-        <v>35</v>
+        <v>13.8</v>
       </c>
       <c r="G8">
-        <v>25</v>
+        <v>9.8</v>
       </c>
       <c r="H8">
         <v>1.04</v>
@@ -624,13 +624,13 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>42</v>
+        <v>16.5</v>
       </c>
       <c r="F9">
-        <v>30</v>
+        <v>11.8</v>
       </c>
       <c r="G9">
-        <v>20</v>
+        <v>7.9</v>
       </c>
       <c r="H9">
         <v>0.48</v>

</xml_diff>